<commit_message>
Commiting Login module, hooks, LoginSer,LoginReq, ConfigMgr, ReqBuild,RespBuild,Context, TokenMgr
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anand\IdeaProjects\team4_api_guardians\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Team04_API_Guardians\git_Team04\team4_api_guardians\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5FE53B-E43D-4CC9-8554-DBE93C83AA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C26BC2-0283-430B-B9AC-FBBF0E15FE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
-  <si>
-    <t>Body</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>EndPoint</t>
   </si>
@@ -69,9 +66,6 @@
     <t>InvalidData</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Skill</t>
   </si>
   <si>
@@ -118,13 +112,67 @@
   </si>
   <si>
     <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>HTTPMethod</t>
+  </si>
+  <si>
+    <t>ContentType</t>
+  </si>
+  <si>
+    <t>ExpectedStatus</t>
+  </si>
+  <si>
+    <t>ExpectedMessage</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>ApiHackathon2@4</t>
+  </si>
+  <si>
+    <t>team4@gmail.com</t>
+  </si>
+  <si>
+    <t>application/xml</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>TC04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,16 +180,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,14 +229,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,40 +593,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D495E3D-B3D5-4AFB-9134-10A138B201AB}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" customWidth="1"/>
-    <col min="4" max="4" width="24.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1">
+        <v>201</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1">
+        <v>405</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1">
+        <v>400</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1">
+        <v>415</v>
+      </c>
+      <c r="H5" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{25F07481-86BF-44A3-9402-6F2F831DCFFA}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{9AE6EF2F-7062-49CE-8707-B36EE749EC54}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{CE0DEEEE-E206-4860-AD36-2006D2CA7F06}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{4CAC2AD7-91B3-4B31-96BC-2DCF2CADA0DE}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{3CFCD072-ECDB-49ED-9CEA-D724F79E4129}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{824D2793-0D2B-4B86-90AC-F855D23897D3}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{52178F12-577B-4275-B4A6-539742D73472}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{6DADF24F-8F4C-4CAF-AF57-074592C96E58}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -531,44 +755,44 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -580,90 +804,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3203F916-7C5D-43BD-85A4-1BC738372894}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>14</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>18</v>
       </c>
       <c r="B8">
         <v>444</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>555</v>
@@ -680,7 +902,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -694,11 +916,11 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nishi created feature file, stepdefinition and log4j files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anand\IdeaProjects\team4_api_guardians\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\team4_api_guardians\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E3BF64-0B71-47A5-B24B-92BB30B32FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE3333F-F760-4178-8BBC-7D52FE2C1F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>Body</t>
   </si>
@@ -54,21 +54,6 @@
     <t>StatusCode</t>
   </si>
   <si>
-    <t>TestCase_Id</t>
-  </si>
-  <si>
-    <t>StatusMessage</t>
-  </si>
-  <si>
-    <t>RequestBody</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>InvalidData</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -184,6 +169,45 @@
   </si>
   <si>
     <t>Data Science</t>
+  </si>
+  <si>
+    <t>Program Status</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/saveprogram</t>
+  </si>
+  <si>
+    <t>Program Description</t>
+  </si>
+  <si>
+    <t>CreateProgram</t>
+  </si>
+  <si>
+    <t>Old ABC</t>
+  </si>
+  <si>
+    <t>Flower Botany</t>
+  </si>
+  <si>
+    <t>CreateProgramWitoutAuthoriztion</t>
+  </si>
+  <si>
+    <t>Music Classic</t>
+  </si>
+  <si>
+    <t>Music New</t>
+  </si>
+  <si>
+    <t>CreateProgramWithValidLengthProgramDescription</t>
+  </si>
+  <si>
+    <t>First new program started</t>
+  </si>
+  <si>
+    <t>Acting New</t>
   </si>
 </sst>
 </file>
@@ -572,7 +596,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -594,47 +618,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE2ED4C-7CD9-4EDB-8F03-B445C483B80C}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.90625" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
     <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -646,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3203F916-7C5D-43BD-85A4-1BC738372894}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,283 +747,283 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>444</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>555</v>
       </c>
       <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G14">
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J16" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -975,7 +1056,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing RestAssuredUtil for HTTP Calls, LoginSteps, Testdata sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Team04_API_Guardians\git_Team04\team4_api_guardians\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C26BC2-0283-430B-B9AC-FBBF0E15FE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6391B68F-81B7-4418-82BD-BF663B316C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="2" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>EndPoint</t>
   </si>
@@ -141,12 +141,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>application/json</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
     <t>ApiHackathon2@4</t>
   </si>
   <si>
@@ -166,6 +160,36 @@
   </si>
   <si>
     <t>TC04</t>
+  </si>
+  <si>
+    <t>/loginUser</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>tea@#$%m4@gma#$%il.com</t>
+  </si>
+  <si>
+    <t>ApiHackatho!@#$%^&amp;n2@4</t>
+  </si>
+  <si>
+    <t>1234567894@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -249,15 +273,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,19 +618,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D495E3D-B3D5-4AFB-9134-10A138B201AB}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -639,13 +664,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>
@@ -653,9 +678,7 @@
       <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1">
         <v>201</v>
       </c>
@@ -663,37 +686,35 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
@@ -701,9 +722,7 @@
       <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1">
         <v>400</v>
       </c>
@@ -711,13 +730,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>31</v>
@@ -726,27 +745,133 @@
         <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1">
         <v>415</v>
       </c>
       <c r="H5" s="1"/>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6">
+        <v>123456789</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{25F07481-86BF-44A3-9402-6F2F831DCFFA}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{9AE6EF2F-7062-49CE-8707-B36EE749EC54}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{CE0DEEEE-E206-4860-AD36-2006D2CA7F06}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{4CAC2AD7-91B3-4B31-96BC-2DCF2CADA0DE}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{3CFCD072-ECDB-49ED-9CEA-D724F79E4129}"/>
-    <hyperlink ref="C3" r:id="rId6" xr:uid="{824D2793-0D2B-4B86-90AC-F855D23897D3}"/>
-    <hyperlink ref="C4" r:id="rId7" xr:uid="{52178F12-577B-4275-B4A6-539742D73472}"/>
-    <hyperlink ref="C5" r:id="rId8" xr:uid="{6DADF24F-8F4C-4CAF-AF57-074592C96E58}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -804,7 +929,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3203F916-7C5D-43BD-85A4-1BC738372894}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
commiting optimized code for User login
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Team04_API_Guardians\git_Team04\team4_api_guardians\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6391B68F-81B7-4418-82BD-BF663B316C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F57FB06-B27C-48D7-A81F-663F2DDE4576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="2" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>EndPoint</t>
   </si>
@@ -190,6 +190,36 @@
   </si>
   <si>
     <t>1234567894@gmail.com</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>invalid@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -273,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -281,8 +311,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -618,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D495E3D-B3D5-4AFB-9134-10A138B201AB}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,13 +697,13 @@
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -688,21 +719,20 @@
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1">
-        <v>401</v>
+      <c r="D3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3">
+        <v>405</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -710,21 +740,17 @@
       <c r="A4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1">
-        <v>400</v>
+      <c r="D4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -732,13 +758,13 @@
       <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -748,7 +774,7 @@
         <v>35</v>
       </c>
       <c r="G5" s="1">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -756,31 +782,33 @@
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>400</v>
+      </c>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="6">
-        <v>123456789</v>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>31</v>
@@ -789,17 +817,21 @@
         <v>32</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>415</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
@@ -814,8 +846,10 @@
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -832,11 +866,11 @@
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>33</v>
+      <c r="C10" s="5">
+        <v>123456789</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>31</v>
@@ -852,12 +886,10 @@
       <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
@@ -867,6 +899,150 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -929,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3203F916-7C5D-43BD-85A4-1BC738372894}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Committing hooks, loginservice, SessonManager, TesContext, LoginFeature
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Team04_API_Guardians\git_Team04\team4_api_guardians\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F57FB06-B27C-48D7-A81F-663F2DDE4576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037735D8-6536-4986-A4B3-A5DCC98DE295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="3" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
   <si>
     <t>EndPoint</t>
   </si>
@@ -219,14 +219,107 @@
     <t>GET</t>
   </si>
   <si>
-    <t>invalid@gmail.com</t>
+    <t>userComments</t>
+  </si>
+  <si>
+    <t>userEduPg</t>
+  </si>
+  <si>
+    <t>userEduUg</t>
+  </si>
+  <si>
+    <t>userFirstName</t>
+  </si>
+  <si>
+    <t>userLastName</t>
+  </si>
+  <si>
+    <t>userLinkedinUrl</t>
+  </si>
+  <si>
+    <t>userLocation</t>
+  </si>
+  <si>
+    <t>userTimeZone</t>
+  </si>
+  <si>
+    <t>userVisaStatus</t>
+  </si>
+  <si>
+    <t>roleId</t>
+  </si>
+  <si>
+    <t>userRoleStatus</t>
+  </si>
+  <si>
+    <t>userLoginEmail</t>
+  </si>
+  <si>
+    <t>loginStatus</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>H1B</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>/users/roleStatus</t>
+  </si>
+  <si>
+    <t>smith</t>
+  </si>
+  <si>
+    <t>test comments</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>www.linkedin.com</t>
+  </si>
+  <si>
+    <t>/users/</t>
+  </si>
+  <si>
+    <t>userPhoneNumber</t>
+  </si>
+  <si>
+    <t>+91 7944540236</t>
+  </si>
+  <si>
+    <t>Ginny</t>
+  </si>
+  <si>
+    <t>abc4@gmail.com</t>
+  </si>
+  <si>
+    <t>/login/forgotpassword/confirmEmail</t>
+  </si>
+  <si>
+    <t>invalid$gmail.com</t>
+  </si>
+  <si>
+    <t>/login/forgotpassword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +345,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -303,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -313,7 +412,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -649,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D495E3D-B3D5-4AFB-9134-10A138B201AB}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +768,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -938,14 +1046,12 @@
       <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>32</v>
@@ -958,14 +1064,12 @@
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>32</v>
@@ -979,13 +1083,11 @@
         <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>32</v>
@@ -998,10 +1100,12 @@
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>32</v>
@@ -1014,21 +1118,15 @@
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
@@ -1036,13 +1134,25 @@
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1106,7 +1216,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,12 +1311,152 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA50047-0086-4722-99E0-3C1A8D205CF2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{41567574-CE0D-4242-B0AC-351EE13002C2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
integrated modules batch & login
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anand\IdeaProjects\team4_api_guardians\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6D3FDC-7E38-461C-A943-7B74B5051EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402EE55F-9284-4D2E-9080-E3F532A740F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="65">
-  <si>
-    <t>Body</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="97">
   <si>
     <t>EndPoint</t>
   </si>
@@ -69,9 +66,6 @@
     <t>InvalidData</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Skill</t>
   </si>
   <si>
@@ -235,13 +229,115 @@
   </si>
   <si>
     <t>new batch</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>HTTPMethod</t>
+  </si>
+  <si>
+    <t>ContentType</t>
+  </si>
+  <si>
+    <t>ExpectedStatus</t>
+  </si>
+  <si>
+    <t>ExpectedMessage</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>team4@gmail.com</t>
+  </si>
+  <si>
+    <t>ApiHackathon2@4</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>application/xml</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>/loginUser</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>tea@#$%m4@gma#$%il.com</t>
+  </si>
+  <si>
+    <t>TC07</t>
+  </si>
+  <si>
+    <t>ApiHackatho!@#$%^&amp;n2@4</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>1234567894@gmail.com</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>TC11</t>
+  </si>
+  <si>
+    <t>TC12</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>invalid@gmail.com</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>TC18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,16 +345,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -266,14 +388,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D495E3D-B3D5-4AFB-9134-10A138B201AB}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,22 +769,385 @@
     <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <v>201</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>405</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="2">
+        <v>401</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>400</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>415</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="6">
+        <v>123456789</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -664,28 +1175,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -697,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3203F916-7C5D-43BD-85A4-1BC738372894}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -717,91 +1228,91 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
       <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>444</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K4">
         <v>444</v>
@@ -809,127 +1320,127 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11">
         <v>555</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K11">
         <v>555</v>
@@ -937,53 +1448,53 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>888</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K14">
         <v>888</v>
@@ -991,83 +1502,83 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G16">
         <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>224</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17">
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K17">
         <v>224</v>
@@ -1075,71 +1586,71 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18">
         <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19">
         <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E19">
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>98</v>
@@ -1148,92 +1659,92 @@
         <v>1234</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21">
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G21">
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22">
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1266,7 +1777,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for user login module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Team04_API_Guardians\git_Team04\team4_api_guardians\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037735D8-6536-4986-A4B3-A5DCC98DE295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5A756C-D278-42C9-927D-706B7C70D16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="3" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="2" xr2:uid="{97D18A69-7170-4542-86C9-C7E18D31EAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
@@ -40,35 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="209">
   <si>
     <t>EndPoint</t>
   </si>
   <si>
-    <t>RequestName</t>
-  </si>
-  <si>
-    <t>StatusCode</t>
-  </si>
-  <si>
-    <t>TestCase_Id</t>
-  </si>
-  <si>
-    <t>StatusMessage</t>
-  </si>
-  <si>
-    <t>RequestBody</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>InvalidData</t>
-  </si>
-  <si>
-    <t>Skill</t>
-  </si>
-  <si>
     <t>Batch ID</t>
   </si>
   <si>
@@ -78,33 +54,6 @@
     <t>Program ID</t>
   </si>
   <si>
-    <t>Valid Batch ID Generic</t>
-  </si>
-  <si>
-    <t>Valid Batch Name Generic</t>
-  </si>
-  <si>
-    <t>Valid Batch ID from Create</t>
-  </si>
-  <si>
-    <t>Valid Batch Name from Create</t>
-  </si>
-  <si>
-    <t>Invalid Batch ID</t>
-  </si>
-  <si>
-    <t>Invalid Batch Name</t>
-  </si>
-  <si>
-    <t>Valid Program ID Generic</t>
-  </si>
-  <si>
-    <t>Valid Program ID from Create</t>
-  </si>
-  <si>
-    <t>Invalid Program ID</t>
-  </si>
-  <si>
     <t>DA02</t>
   </si>
   <si>
@@ -313,13 +262,418 @@
   </si>
   <si>
     <t>/login/forgotpassword</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>TC19</t>
+  </si>
+  <si>
+    <t>TC20</t>
+  </si>
+  <si>
+    <t>TC21</t>
+  </si>
+  <si>
+    <t>TC22</t>
+  </si>
+  <si>
+    <t>TC23</t>
+  </si>
+  <si>
+    <t>TC24</t>
+  </si>
+  <si>
+    <t>/logoutlms</t>
+  </si>
+  <si>
+    <t>/logoutinvalid</t>
+  </si>
+  <si>
+    <t>TC25</t>
+  </si>
+  <si>
+    <t>TC26</t>
+  </si>
+  <si>
+    <t>TC27</t>
+  </si>
+  <si>
+    <t>TC28</t>
+  </si>
+  <si>
+    <t>TC29</t>
+  </si>
+  <si>
+    <t>TC30</t>
+  </si>
+  <si>
+    <t>TC31</t>
+  </si>
+  <si>
+    <t>TC32</t>
+  </si>
+  <si>
+    <t>/resetPassword</t>
+  </si>
+  <si>
+    <t>ApiHac2423423n2@4</t>
+  </si>
+  <si>
+    <t>/resetPass</t>
+  </si>
+  <si>
+    <t>james@gmail.com</t>
+  </si>
+  <si>
+    <t>ApiHackathhj2@4</t>
+  </si>
+  <si>
+    <t>tea4@gmail.com</t>
+  </si>
+  <si>
+    <t>team@gmail.com</t>
+  </si>
+  <si>
+    <t>tm4@gmail.com</t>
+  </si>
+  <si>
+    <t>teamk4@gmail.com</t>
+  </si>
+  <si>
+    <t>teah4@gmail.com</t>
+  </si>
+  <si>
+    <t>oiuy@gmail.com</t>
+  </si>
+  <si>
+    <t>skillName</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>skillId</t>
+  </si>
+  <si>
+    <t>creationTime</t>
+  </si>
+  <si>
+    <t>myskill</t>
+  </si>
+  <si>
+    <t>/SaveSkillMaster</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Valid fields</t>
+  </si>
+  <si>
+    <t>Batch Status</t>
+  </si>
+  <si>
+    <t>Program Name</t>
+  </si>
+  <si>
+    <t>Batch No of Classes</t>
+  </si>
+  <si>
+    <t>Request Type</t>
+  </si>
+  <si>
+    <t>Path Param</t>
+  </si>
+  <si>
+    <t>Error Value</t>
+  </si>
+  <si>
+    <t>Get Valid Batch ID Generic</t>
+  </si>
+  <si>
+    <t>/batches/batchId/{batchId}</t>
+  </si>
+  <si>
+    <t>Get Valid Batch ID after delete</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Get Invalid Batch ID</t>
+  </si>
+  <si>
+    <t>Get Valid Batch ID with invalid endpoint</t>
+  </si>
+  <si>
+    <t>/batch/batchId/{batchId}</t>
+  </si>
+  <si>
+    <t>Get Valid Batch Name Generic</t>
+  </si>
+  <si>
+    <t>API Guardians</t>
+  </si>
+  <si>
+    <t>/batches/batchName/{batchName}</t>
+  </si>
+  <si>
+    <t>Get Invalid Batch Name</t>
+  </si>
+  <si>
+    <t>Get Valid Batch Name after delete</t>
+  </si>
+  <si>
+    <t>VERONING</t>
+  </si>
+  <si>
+    <t>Get Valid Batch Name with invalid endpoint</t>
+  </si>
+  <si>
+    <t>/batch/batchName/{batchName}</t>
+  </si>
+  <si>
+    <t>Get Valid Program ID Generic</t>
+  </si>
+  <si>
+    <t>/batches/program/{programId}</t>
+  </si>
+  <si>
+    <t>Get Invalid Program ID</t>
+  </si>
+  <si>
+    <t>Get Program ID with invalid endpoint</t>
+  </si>
+  <si>
+    <t>/batch/program/{programId}</t>
+  </si>
+  <si>
+    <t>Get batch with deleted programId</t>
+  </si>
+  <si>
+    <t>Delete Valid Batch ID Generic</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>/batches/{batchId}</t>
+  </si>
+  <si>
+    <t>Delete Invalid Batch ID</t>
+  </si>
+  <si>
+    <t>Delete batch with invalid endpoint</t>
+  </si>
+  <si>
+    <t>/batch/{batchId}</t>
+  </si>
+  <si>
+    <t>Put Valid Batch ID Generic</t>
+  </si>
+  <si>
+    <t>Batch01</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Put Invalid Batch ID</t>
+  </si>
+  <si>
+    <t>Put Batch ID with missing batchName</t>
+  </si>
+  <si>
+    <t>SDET2</t>
+  </si>
+  <si>
+    <t>Put Batch ID with missing batchStatus</t>
+  </si>
+  <si>
+    <t>bsc test</t>
+  </si>
+  <si>
+    <t>tatus</t>
+  </si>
+  <si>
+    <t>Put Batch with invalid data</t>
+  </si>
+  <si>
+    <t>Put Batch with invalid endpoint</t>
+  </si>
+  <si>
+    <t>Put Batch with deleted batchId</t>
+  </si>
+  <si>
+    <t>new batch</t>
+  </si>
+  <si>
+    <t>Put Valid batchId with deleted programId</t>
+  </si>
+  <si>
+    <t>Batch04</t>
+  </si>
+  <si>
+    <t>Stringg</t>
+  </si>
+  <si>
+    <t>Get all batches</t>
+  </si>
+  <si>
+    <t>/batches</t>
+  </si>
+  <si>
+    <t>Get all batches with invalid endpoint</t>
+  </si>
+  <si>
+    <t>/batch</t>
+  </si>
+  <si>
+    <t>Create New Batch</t>
+  </si>
+  <si>
+    <t>Nnnbatch</t>
+  </si>
+  <si>
+    <t>Program Description</t>
+  </si>
+  <si>
+    <t>Program Status</t>
+  </si>
+  <si>
+    <t>CreateProgram</t>
+  </si>
+  <si>
+    <t>Test Program</t>
+  </si>
+  <si>
+    <t>Life Science</t>
+  </si>
+  <si>
+    <t>/saveprogram</t>
+  </si>
+  <si>
+    <t>CreateProgramWitoutAuthoriztion</t>
+  </si>
+  <si>
+    <t>Music Classic</t>
+  </si>
+  <si>
+    <t>Music New</t>
+  </si>
+  <si>
+    <t>CreateProgramWithValidLengthProgramDescription</t>
+  </si>
+  <si>
+    <t>First new program started</t>
+  </si>
+  <si>
+    <t>Acting New</t>
+  </si>
+  <si>
+    <t>CreateProgramValidLengthProgramName</t>
+  </si>
+  <si>
+    <t>Water Purification</t>
+  </si>
+  <si>
+    <t>Second New Program begin</t>
+  </si>
+  <si>
+    <t>CreateProgramInvalidEndPoint</t>
+  </si>
+  <si>
+    <t>Air Cleaning</t>
+  </si>
+  <si>
+    <t>Enviornment Science</t>
+  </si>
+  <si>
+    <t>CreateProgramExistingAlready</t>
+  </si>
+  <si>
+    <t>Land Cultivation</t>
+  </si>
+  <si>
+    <t>CreateProgramWrongMethod</t>
+  </si>
+  <si>
+    <t>Cooking Beginer</t>
+  </si>
+  <si>
+    <t>Home Science</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>CreateProgramInvalidBody</t>
+  </si>
+  <si>
+    <t>Beginer Dancing</t>
+  </si>
+  <si>
+    <t>Dance and Art</t>
+  </si>
+  <si>
+    <t>CreateProgramMissingValues</t>
+  </si>
+  <si>
+    <t>Singing Classes</t>
+  </si>
+  <si>
+    <t>Singing</t>
+  </si>
+  <si>
+    <t>CreateProgramMissingAdditionalValues</t>
+  </si>
+  <si>
+    <t>Hindi Classes</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>RetrieveAllProgramsValidEndpoint</t>
+  </si>
+  <si>
+    <t>/allPrograms</t>
+  </si>
+  <si>
+    <t>RetrieveAllProgramsInvalidEndPoint</t>
+  </si>
+  <si>
+    <t>RetrieveAllProgramsInvalidMethod</t>
+  </si>
+  <si>
+    <t>RetrieveAllProgramsWithoutAuthorization</t>
+  </si>
+  <si>
+    <t>RetrieveProgramValidID</t>
+  </si>
+  <si>
+    <t>/programs/{programId}</t>
+  </si>
+  <si>
+    <t>RetrieveProgramInvalidID</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,8 +707,16 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,8 +735,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -397,12 +771,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -422,6 +826,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -757,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D495E3D-B3D5-4AFB-9134-10A138B201AB}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,45 +1201,45 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
@@ -825,19 +1249,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="G3">
         <v>405</v>
@@ -846,40 +1270,40 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1">
         <v>401</v>
@@ -888,19 +1312,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1">
@@ -910,19 +1334,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1">
@@ -932,19 +1356,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -952,19 +1376,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -972,19 +1396,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C10" s="5">
         <v>123456789</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -992,17 +1416,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1010,17 +1434,17 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1028,15 +1452,15 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1044,17 +1468,17 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1062,17 +1486,17 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1080,17 +1504,17 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1098,17 +1522,17 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1116,15 +1540,15 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1132,79 +1556,803 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{27A9E3D3-FD48-40F1-B15B-D723B80D7101}"/>
+    <hyperlink ref="B27" r:id="rId2" xr:uid="{BF87A68E-8562-4930-B5B6-F7371E6F3B74}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{106029BD-001A-46D3-9608-A52CA0625CD1}"/>
+    <hyperlink ref="B29" r:id="rId4" xr:uid="{B2976082-168F-49E8-8BA0-3A603874E292}"/>
+    <hyperlink ref="B30" r:id="rId5" xr:uid="{44E3CA92-E857-462F-BBA9-9E5D3DB0D239}"/>
+    <hyperlink ref="B31" r:id="rId6" xr:uid="{19039804-AA52-4199-9F57-979FCA4281CF}"/>
+    <hyperlink ref="B32" r:id="rId7" xr:uid="{CC77B09E-0259-40E8-AF10-9734D180E7FD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE2ED4C-7CD9-4EDB-8F03-B445C483B80C}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1213,96 +2361,754 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3203F916-7C5D-43BD-85A4-1BC738372894}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
+      <c r="J1" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="20">
+        <v>274</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="20">
+        <v>86</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="20"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="20">
+        <v>444</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="20">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="20">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20">
+        <v>3</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20">
+        <v>555</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="20">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20">
+        <v>3</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20">
+        <v>49</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="20">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="20">
+        <v>88</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="20">
+        <v>888</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="20">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="20">
+        <v>88</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="20">
+        <v>24</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="20">
+        <v>2</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G17" s="20">
+        <v>8</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="20">
+        <v>2024</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="20">
+        <v>2</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" s="20">
+        <v>8</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="20">
+        <v>98</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="20">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
+      <c r="F19" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="20">
+        <v>1</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="20">
+        <v>98</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20">
+        <v>13</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="20">
+        <v>98</v>
+      </c>
+      <c r="C21" s="20">
+        <v>1234</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="20">
+        <v>13</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="20">
+        <v>1</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="20">
+        <v>24</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="20">
+        <v>2</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="20">
+        <v>8</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="20">
+        <v>86</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="20">
+        <v>13</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="20">
+        <v>1</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="20">
+        <v>98</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="20">
+        <v>49</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" s="20">
+        <v>1</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="20">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>555</v>
-      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20">
+        <v>1</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1313,7 +3119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA50047-0086-4722-99E0-3C1A8D205CF2}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -1340,116 +3146,116 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="Q1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="N2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="Q2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="O3" s="10"/>
     </row>
@@ -1463,18 +3269,85 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E93E2C-CF83-4E2D-B38A-8B7ED372BA16}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="19">
+        <v>201</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>